<commit_message>
fix inserts into region_incomes
</commit_message>
<xml_diff>
--- a/files/regions.xlsx
+++ b/files/regions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\projects\AverageRegionIncomes\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD6ECE8-D054-4316-949D-0B2D1635A7F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366E8943-2F17-424C-8596-5385FF5254CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5CD539C1-DC06-4AB2-B73B-34E35F85C80F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5CD539C1-DC06-4AB2-B73B-34E35F85C80F}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -700,20 +700,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEEB42CB-F95F-4E74-9151-79FBCDFA3549}">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
@@ -721,676 +721,1012 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="str">
+        <f>CONCATENATE("(",A2,",","'",B2,"'",")")</f>
+        <v>(1,'Республика Адыгея  ')</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="str">
+        <f t="shared" ref="C3:C66" si="0">CONCATENATE("(",A3,",","'",B3,"'",")")</f>
+        <v>(2,'Республика Башкортостан')</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,'Республика Бурятия')</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,'Республика Алтай')</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,'Республика Дагестан')</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,'Республика Ингушетия')</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,'Кабардино-Балкарская  Республика')</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,'Республика Калмыкия')</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,'Карачаево-Черкесская  Республика')</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,'Республика Карелия')</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,'Республика Коми')</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,'Республика Марий Эл  ')</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,'Республика Мордовия')</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,'Республика Саха (Якутия)')</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,'Республика  Северная Осетия - Алания')</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,'Республика Татарстан')</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(17,'Республика Тыва')</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(18,'Удмуртская Республика')</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(19,'Республика Хакасия')</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(20,'Чеченская Республика')</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(21,'Чувашская Республика ')</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(22,'Алтайский край')</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(23,'Краснодарский край')</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(24,'Красноярский край   ')</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(25,'Приморский край')</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(26,'Ставропольский край')</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(27,'Хабаровский край ')</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(28,'Амурская область')</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(29,'Архангельская область   ')</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(30,'Астраханская область')</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(31,'Белгородская область  ')</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(32,'Брянская область ')</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(33,'Владимирская область')</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(34,'Волгоградская область')</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(35,'Вологодская область')</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(36,'Воронежская область')</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(37,'Ивановская область')</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(38,'Иркутская область')</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(39,'Калининградская область')</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(40,'Калужская область')</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(41,'Камчатский край   ')</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(42,'Кемеровская область')</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(43,'Кировская область')</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(44,'Костромская область ')</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(45,'Курганская область')</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(46,'Курская область')</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(47,'Ленинградская область ')</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(48,'Липецкая область')</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(49,'Магаданская область ')</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(50,'Московская область')</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(51,'Мурманская область   ')</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(52,'Нижегородская область ')</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(53,'Новгородская область')</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(54,'Новосибирская область')</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(55,'Омская область')</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(56,'Оренбургская область')</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(57,'Орловская область')</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(58,'Пензенская область ')</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(59,'Пермский край')</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(60,'Псковская область   ')</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(61,'Ростовская область ')</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(62,'Рязанская область')</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(63,'Самарская область')</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(64,'Саратовская область')</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(65,'Сахалинская область   ')</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67" s="1" t="str">
+        <f t="shared" ref="C67:C85" si="1">CONCATENATE("(",A67,",","'",B67,"'",")")</f>
+        <v>(66,'Свердловская область')</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(67,'Смоленская область')</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(68,'Тамбовская область ')</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(69,'Тверская область')</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(70,'Томская область')</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(71,'Тульская область')</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(72,'Тюменская область   ')</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(73,'Ульяновская область')</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(74,'Челябинская область')</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(75,'Забайкальский край')</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(76,'Ярославская область   ')</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(77,'г.Москва')</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(78,'г.Санкт-Петербург')</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(79,'Еврейская  авт.область')</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>83</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(83,'Ненецкий авт.округ')</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>86</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(86,'Ханты-Мансийский авт.округ')</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>87</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(87,'Чукотский  авт.округ')</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>89</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(89,'Ямало-Ненецкий авт.округ')</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>99</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>50</v>
+      </c>
+      <c r="C85" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(99,'Иные территории, включая город и космодром Байконур')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>